<commit_message>
add holiday and weekend volumes
</commit_message>
<xml_diff>
--- a/passenger_flows/weekend/AlightVolume-30min/alight_9号线-idx-9.xlsx
+++ b/passenger_flows/weekend/AlightVolume-30min/alight_9号线-idx-9.xlsx
@@ -744,106 +744,106 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F3">
+        <v>113</v>
+      </c>
+      <c r="G3">
+        <v>122</v>
+      </c>
+      <c r="H3">
+        <v>123</v>
+      </c>
+      <c r="I3">
+        <v>112</v>
+      </c>
+      <c r="J3">
+        <v>95</v>
+      </c>
+      <c r="K3">
+        <v>68</v>
+      </c>
+      <c r="L3">
+        <v>83</v>
+      </c>
+      <c r="M3">
+        <v>65</v>
+      </c>
+      <c r="N3">
+        <v>58</v>
+      </c>
+      <c r="O3">
+        <v>55</v>
+      </c>
+      <c r="P3">
+        <v>58</v>
+      </c>
+      <c r="Q3">
+        <v>51</v>
+      </c>
+      <c r="R3">
+        <v>51</v>
+      </c>
+      <c r="S3">
+        <v>55</v>
+      </c>
+      <c r="T3">
+        <v>45</v>
+      </c>
+      <c r="U3">
+        <v>45</v>
+      </c>
+      <c r="V3">
+        <v>41</v>
+      </c>
+      <c r="W3">
+        <v>40</v>
+      </c>
+      <c r="X3">
+        <v>37</v>
+      </c>
+      <c r="Y3">
+        <v>42</v>
+      </c>
+      <c r="Z3">
+        <v>67</v>
+      </c>
+      <c r="AA3">
+        <v>117</v>
+      </c>
+      <c r="AB3">
         <v>118</v>
       </c>
-      <c r="G3">
-        <v>128</v>
-      </c>
-      <c r="H3">
-        <v>128</v>
-      </c>
-      <c r="I3">
-        <v>118</v>
-      </c>
-      <c r="J3">
-        <v>99</v>
-      </c>
-      <c r="K3">
-        <v>70</v>
-      </c>
-      <c r="L3">
-        <v>124</v>
-      </c>
-      <c r="M3">
-        <v>95</v>
-      </c>
-      <c r="N3">
-        <v>87</v>
-      </c>
-      <c r="O3">
-        <v>83</v>
-      </c>
-      <c r="P3">
-        <v>86</v>
-      </c>
-      <c r="Q3">
-        <v>77</v>
-      </c>
-      <c r="R3">
+      <c r="AC3">
+        <v>68</v>
+      </c>
+      <c r="AD3">
         <v>76</v>
       </c>
-      <c r="S3">
-        <v>83</v>
-      </c>
-      <c r="T3">
-        <v>67</v>
-      </c>
-      <c r="U3">
-        <v>68</v>
-      </c>
-      <c r="V3">
-        <v>63</v>
-      </c>
-      <c r="W3">
-        <v>59</v>
-      </c>
-      <c r="X3">
-        <v>56</v>
-      </c>
-      <c r="Y3">
-        <v>62</v>
-      </c>
-      <c r="Z3">
-        <v>70</v>
-      </c>
-      <c r="AA3">
-        <v>122</v>
-      </c>
-      <c r="AB3">
-        <v>122</v>
-      </c>
-      <c r="AC3">
-        <v>70</v>
-      </c>
-      <c r="AD3">
-        <v>78</v>
-      </c>
       <c r="AE3">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF3">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AG3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AI3">
         <v>23</v>
       </c>
       <c r="AJ3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AK3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL3">
         <v>8</v>
@@ -863,109 +863,109 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F4">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G4">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H4">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I4">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J4">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K4">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L4">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="M4">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N4">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="O4">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="P4">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="Q4">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="R4">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="S4">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="T4">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="U4">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="V4">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="W4">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="X4">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="Y4">
+        <v>39</v>
+      </c>
+      <c r="Z4">
+        <v>64</v>
+      </c>
+      <c r="AA4">
+        <v>111</v>
+      </c>
+      <c r="AB4">
+        <v>113</v>
+      </c>
+      <c r="AC4">
+        <v>66</v>
+      </c>
+      <c r="AD4">
+        <v>118</v>
+      </c>
+      <c r="AE4">
+        <v>111</v>
+      </c>
+      <c r="AF4">
+        <v>92</v>
+      </c>
+      <c r="AG4">
+        <v>74</v>
+      </c>
+      <c r="AH4">
         <v>58</v>
       </c>
-      <c r="Z4">
-        <v>67</v>
-      </c>
-      <c r="AA4">
-        <v>116</v>
-      </c>
-      <c r="AB4">
-        <v>116</v>
-      </c>
-      <c r="AC4">
-        <v>67</v>
-      </c>
-      <c r="AD4">
-        <v>121</v>
-      </c>
-      <c r="AE4">
-        <v>115</v>
-      </c>
-      <c r="AF4">
-        <v>95</v>
-      </c>
-      <c r="AG4">
-        <v>78</v>
-      </c>
-      <c r="AH4">
-        <v>60</v>
-      </c>
       <c r="AI4">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AJ4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AL4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AM4">
         <v>5</v>
@@ -982,106 +982,106 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F5">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G5">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H5">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I5">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="J5">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K5">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L5">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="M5">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="N5">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="O5">
+        <v>27</v>
+      </c>
+      <c r="P5">
+        <v>30</v>
+      </c>
+      <c r="Q5">
+        <v>33</v>
+      </c>
+      <c r="R5">
+        <v>32</v>
+      </c>
+      <c r="S5">
+        <v>32</v>
+      </c>
+      <c r="T5">
         <v>40</v>
       </c>
-      <c r="P5">
-        <v>45</v>
-      </c>
-      <c r="Q5">
+      <c r="U5">
+        <v>35</v>
+      </c>
+      <c r="V5">
+        <v>38</v>
+      </c>
+      <c r="W5">
+        <v>41</v>
+      </c>
+      <c r="X5">
         <v>49</v>
       </c>
-      <c r="R5">
-        <v>47</v>
-      </c>
-      <c r="S5">
-        <v>48</v>
-      </c>
-      <c r="T5">
+      <c r="Y5">
+        <v>63</v>
+      </c>
+      <c r="Z5">
+        <v>96</v>
+      </c>
+      <c r="AA5">
+        <v>169</v>
+      </c>
+      <c r="AB5">
+        <v>170</v>
+      </c>
+      <c r="AC5">
+        <v>95</v>
+      </c>
+      <c r="AD5">
+        <v>177</v>
+      </c>
+      <c r="AE5">
+        <v>175</v>
+      </c>
+      <c r="AF5">
+        <v>155</v>
+      </c>
+      <c r="AG5">
+        <v>123</v>
+      </c>
+      <c r="AH5">
+        <v>115</v>
+      </c>
+      <c r="AI5">
+        <v>97</v>
+      </c>
+      <c r="AJ5">
+        <v>83</v>
+      </c>
+      <c r="AK5">
         <v>58</v>
-      </c>
-      <c r="U5">
-        <v>52</v>
-      </c>
-      <c r="V5">
-        <v>56</v>
-      </c>
-      <c r="W5">
-        <v>59</v>
-      </c>
-      <c r="X5">
-        <v>74</v>
-      </c>
-      <c r="Y5">
-        <v>95</v>
-      </c>
-      <c r="Z5">
-        <v>100</v>
-      </c>
-      <c r="AA5">
-        <v>174</v>
-      </c>
-      <c r="AB5">
-        <v>174</v>
-      </c>
-      <c r="AC5">
-        <v>100</v>
-      </c>
-      <c r="AD5">
-        <v>182</v>
-      </c>
-      <c r="AE5">
-        <v>182</v>
-      </c>
-      <c r="AF5">
-        <v>162</v>
-      </c>
-      <c r="AG5">
-        <v>130</v>
-      </c>
-      <c r="AH5">
-        <v>117</v>
-      </c>
-      <c r="AI5">
-        <v>100</v>
-      </c>
-      <c r="AJ5">
-        <v>85</v>
-      </c>
-      <c r="AK5">
-        <v>60</v>
       </c>
       <c r="AL5">
         <v>23</v>
@@ -1101,106 +1101,106 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F6">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G6">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H6">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I6">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J6">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K6">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L6">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="M6">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="N6">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="O6">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="P6">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="Q6">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="R6">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="S6">
+        <v>33</v>
+      </c>
+      <c r="T6">
+        <v>34</v>
+      </c>
+      <c r="U6">
+        <v>37</v>
+      </c>
+      <c r="V6">
+        <v>33</v>
+      </c>
+      <c r="W6">
+        <v>34</v>
+      </c>
+      <c r="X6">
         <v>48</v>
       </c>
-      <c r="T6">
-        <v>50</v>
-      </c>
-      <c r="U6">
-        <v>55</v>
-      </c>
-      <c r="V6">
-        <v>50</v>
-      </c>
-      <c r="W6">
-        <v>50</v>
-      </c>
-      <c r="X6">
-        <v>71</v>
-      </c>
       <c r="Y6">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="Z6">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AA6">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AB6">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AC6">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AD6">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AE6">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AF6">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AG6">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="AH6">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AI6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AJ6">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AK6">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AL6">
         <v>25</v>
@@ -1220,109 +1220,109 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E7">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="F7">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="G7">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="H7">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="I7">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="J7">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="K7">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L7">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="M7">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="N7">
-        <v>160</v>
+        <v>106</v>
       </c>
       <c r="O7">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="P7">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="Q7">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="R7">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="S7">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="T7">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="U7">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="V7">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="W7">
-        <v>178</v>
+        <v>123</v>
       </c>
       <c r="X7">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="Y7">
-        <v>226</v>
+        <v>150</v>
       </c>
       <c r="Z7">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="AA7">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="AB7">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="AC7">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AD7">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="AE7">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="AF7">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="AG7">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="AH7">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AI7">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AJ7">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="AK7">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AL7">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AM7">
         <v>5</v>
@@ -1333,115 +1333,115 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>825</v>
+        <v>794</v>
       </c>
       <c r="E8">
-        <v>1162</v>
+        <v>1129</v>
       </c>
       <c r="F8">
-        <v>1387</v>
+        <v>1357</v>
       </c>
       <c r="G8">
-        <v>1499</v>
+        <v>1432</v>
       </c>
       <c r="H8">
-        <v>1499</v>
+        <v>1431</v>
       </c>
       <c r="I8">
-        <v>1387</v>
+        <v>1322</v>
       </c>
       <c r="J8">
-        <v>1162</v>
+        <v>1110</v>
       </c>
       <c r="K8">
-        <v>825</v>
+        <v>802</v>
       </c>
       <c r="L8">
-        <v>1184</v>
+        <v>802</v>
       </c>
       <c r="M8">
-        <v>717</v>
+        <v>485</v>
       </c>
       <c r="N8">
-        <v>748</v>
+        <v>509</v>
       </c>
       <c r="O8">
-        <v>739</v>
+        <v>501</v>
       </c>
       <c r="P8">
-        <v>841</v>
+        <v>571</v>
       </c>
       <c r="Q8">
-        <v>749</v>
+        <v>509</v>
       </c>
       <c r="R8">
-        <v>703</v>
+        <v>476</v>
       </c>
       <c r="S8">
-        <v>819</v>
+        <v>552</v>
       </c>
       <c r="T8">
-        <v>646</v>
+        <v>430</v>
       </c>
       <c r="U8">
-        <v>674</v>
+        <v>458</v>
       </c>
       <c r="V8">
-        <v>749</v>
+        <v>499</v>
       </c>
       <c r="W8">
-        <v>590</v>
+        <v>400</v>
       </c>
       <c r="X8">
-        <v>718</v>
+        <v>488</v>
       </c>
       <c r="Y8">
-        <v>848</v>
+        <v>576</v>
       </c>
       <c r="Z8">
-        <v>825</v>
+        <v>804</v>
       </c>
       <c r="AA8">
-        <v>1437</v>
+        <v>1406</v>
       </c>
       <c r="AB8">
-        <v>1437</v>
+        <v>1379</v>
       </c>
       <c r="AC8">
-        <v>825</v>
+        <v>789</v>
       </c>
       <c r="AD8">
-        <v>1499</v>
+        <v>1439</v>
       </c>
       <c r="AE8">
-        <v>913</v>
+        <v>881</v>
       </c>
       <c r="AF8">
-        <v>774</v>
+        <v>746</v>
       </c>
       <c r="AG8">
-        <v>609</v>
+        <v>583</v>
       </c>
       <c r="AH8">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="AI8">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="AJ8">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="AK8">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="AL8">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AM8">
         <v>11</v>
@@ -1458,109 +1458,109 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="E9">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="F9">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="G9">
-        <v>665</v>
+        <v>641</v>
       </c>
       <c r="H9">
-        <v>665</v>
+        <v>637</v>
       </c>
       <c r="I9">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="J9">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="K9">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="L9">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="M9">
-        <v>246</v>
+        <v>171</v>
       </c>
       <c r="N9">
-        <v>244</v>
+        <v>165</v>
       </c>
       <c r="O9">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="P9">
-        <v>220</v>
+        <v>152</v>
       </c>
       <c r="Q9">
-        <v>229</v>
+        <v>154</v>
       </c>
       <c r="R9">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="S9">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="T9">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="U9">
-        <v>264</v>
+        <v>179</v>
       </c>
       <c r="V9">
-        <v>280</v>
+        <v>185</v>
       </c>
       <c r="W9">
-        <v>300</v>
+        <v>204</v>
       </c>
       <c r="X9">
-        <v>350</v>
+        <v>233</v>
       </c>
       <c r="Y9">
-        <v>435</v>
+        <v>298</v>
       </c>
       <c r="Z9">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="AA9">
-        <v>638</v>
+        <v>619</v>
       </c>
       <c r="AB9">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="AC9">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="AD9">
-        <v>665</v>
+        <v>632</v>
       </c>
       <c r="AE9">
-        <v>665</v>
+        <v>641</v>
       </c>
       <c r="AF9">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="AG9">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="AH9">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="AI9">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="AJ9">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AK9">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="AL9">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM9">
         <v>4</v>
@@ -1571,115 +1571,115 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D10">
-        <v>2344</v>
+        <v>2244</v>
       </c>
       <c r="E10">
-        <v>3301</v>
+        <v>3209</v>
       </c>
       <c r="F10">
-        <v>3939</v>
+        <v>3800</v>
       </c>
       <c r="G10">
-        <v>4258</v>
+        <v>4158</v>
       </c>
       <c r="H10">
-        <v>4258</v>
+        <v>4100</v>
       </c>
       <c r="I10">
-        <v>3939</v>
+        <v>3761</v>
       </c>
       <c r="J10">
-        <v>3301</v>
+        <v>3223</v>
       </c>
       <c r="K10">
-        <v>2344</v>
+        <v>2242</v>
       </c>
       <c r="L10">
-        <v>3228</v>
+        <v>2163</v>
       </c>
       <c r="M10">
-        <v>2883</v>
+        <v>1988</v>
       </c>
       <c r="N10">
-        <v>2776</v>
+        <v>1860</v>
       </c>
       <c r="O10">
-        <v>2537</v>
+        <v>1725</v>
       </c>
       <c r="P10">
-        <v>2845</v>
+        <v>1954</v>
       </c>
       <c r="Q10">
-        <v>2669</v>
+        <v>1783</v>
       </c>
       <c r="R10">
-        <v>2739</v>
+        <v>1855</v>
       </c>
       <c r="S10">
-        <v>2508</v>
+        <v>1669</v>
       </c>
       <c r="T10">
-        <v>2519</v>
+        <v>1695</v>
       </c>
       <c r="U10">
-        <v>2497</v>
+        <v>1691</v>
       </c>
       <c r="V10">
-        <v>2399</v>
+        <v>1615</v>
       </c>
       <c r="W10">
-        <v>2133</v>
+        <v>1444</v>
       </c>
       <c r="X10">
-        <v>2454</v>
+        <v>1630</v>
       </c>
       <c r="Y10">
-        <v>2330</v>
+        <v>1589</v>
       </c>
       <c r="Z10">
-        <v>2344</v>
+        <v>2284</v>
       </c>
       <c r="AA10">
-        <v>4081</v>
+        <v>3918</v>
       </c>
       <c r="AB10">
-        <v>4081</v>
+        <v>3959</v>
       </c>
       <c r="AC10">
-        <v>2344</v>
+        <v>2237</v>
       </c>
       <c r="AD10">
-        <v>2477</v>
+        <v>2416</v>
       </c>
       <c r="AE10">
-        <v>1867</v>
+        <v>1818</v>
       </c>
       <c r="AF10">
-        <v>1476</v>
+        <v>1414</v>
       </c>
       <c r="AG10">
-        <v>1162</v>
+        <v>1104</v>
       </c>
       <c r="AH10">
-        <v>947</v>
+        <v>912</v>
       </c>
       <c r="AI10">
-        <v>717</v>
+        <v>705</v>
       </c>
       <c r="AJ10">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="AK10">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AL10">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AM10">
         <v>24</v>
@@ -1690,115 +1690,115 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="D11">
-        <v>739</v>
+        <v>706</v>
       </c>
       <c r="E11">
-        <v>1041</v>
+        <v>1019</v>
       </c>
       <c r="F11">
-        <v>1242</v>
+        <v>1185</v>
       </c>
       <c r="G11">
-        <v>1342</v>
+        <v>1313</v>
       </c>
       <c r="H11">
-        <v>1342</v>
+        <v>1300</v>
       </c>
       <c r="I11">
-        <v>1242</v>
+        <v>1202</v>
       </c>
       <c r="J11">
-        <v>1041</v>
+        <v>1000</v>
       </c>
       <c r="K11">
-        <v>739</v>
+        <v>722</v>
       </c>
       <c r="L11">
-        <v>1100</v>
+        <v>736</v>
       </c>
       <c r="M11">
-        <v>767</v>
+        <v>527</v>
       </c>
       <c r="N11">
-        <v>872</v>
+        <v>587</v>
       </c>
       <c r="O11">
-        <v>918</v>
+        <v>616</v>
       </c>
       <c r="P11">
-        <v>885</v>
+        <v>594</v>
       </c>
       <c r="Q11">
-        <v>832</v>
+        <v>554</v>
       </c>
       <c r="R11">
-        <v>763</v>
+        <v>506</v>
       </c>
       <c r="S11">
+        <v>484</v>
+      </c>
+      <c r="T11">
+        <v>468</v>
+      </c>
+      <c r="U11">
+        <v>580</v>
+      </c>
+      <c r="V11">
+        <v>495</v>
+      </c>
+      <c r="W11">
+        <v>454</v>
+      </c>
+      <c r="X11">
+        <v>469</v>
+      </c>
+      <c r="Y11">
+        <v>528</v>
+      </c>
+      <c r="Z11">
+        <v>706</v>
+      </c>
+      <c r="AA11">
+        <v>1222</v>
+      </c>
+      <c r="AB11">
+        <v>1254</v>
+      </c>
+      <c r="AC11">
         <v>718</v>
       </c>
-      <c r="T11">
-        <v>694</v>
-      </c>
-      <c r="U11">
-        <v>854</v>
-      </c>
-      <c r="V11">
-        <v>741</v>
-      </c>
-      <c r="W11">
-        <v>672</v>
-      </c>
-      <c r="X11">
-        <v>690</v>
-      </c>
-      <c r="Y11">
-        <v>781</v>
-      </c>
-      <c r="Z11">
-        <v>739</v>
-      </c>
-      <c r="AA11">
-        <v>1286</v>
-      </c>
-      <c r="AB11">
-        <v>1286</v>
-      </c>
-      <c r="AC11">
-        <v>739</v>
-      </c>
       <c r="AD11">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="AE11">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="AF11">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="AG11">
+        <v>315</v>
+      </c>
+      <c r="AH11">
+        <v>290</v>
+      </c>
+      <c r="AI11">
         <v>328</v>
       </c>
-      <c r="AH11">
-        <v>295</v>
-      </c>
-      <c r="AI11">
-        <v>338</v>
-      </c>
       <c r="AJ11">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="AK11">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AL11">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AM11">
         <v>14</v>
@@ -1815,106 +1815,106 @@
         <v>15</v>
       </c>
       <c r="D12">
+        <v>246</v>
+      </c>
+      <c r="E12">
+        <v>353</v>
+      </c>
+      <c r="F12">
+        <v>413</v>
+      </c>
+      <c r="G12">
+        <v>445</v>
+      </c>
+      <c r="H12">
+        <v>452</v>
+      </c>
+      <c r="I12">
+        <v>418</v>
+      </c>
+      <c r="J12">
+        <v>345</v>
+      </c>
+      <c r="K12">
+        <v>246</v>
+      </c>
+      <c r="L12">
+        <v>230</v>
+      </c>
+      <c r="M12">
+        <v>164</v>
+      </c>
+      <c r="N12">
+        <v>159</v>
+      </c>
+      <c r="O12">
+        <v>115</v>
+      </c>
+      <c r="P12">
+        <v>137</v>
+      </c>
+      <c r="Q12">
+        <v>146</v>
+      </c>
+      <c r="R12">
+        <v>162</v>
+      </c>
+      <c r="S12">
+        <v>159</v>
+      </c>
+      <c r="T12">
+        <v>170</v>
+      </c>
+      <c r="U12">
+        <v>175</v>
+      </c>
+      <c r="V12">
+        <v>128</v>
+      </c>
+      <c r="W12">
+        <v>138</v>
+      </c>
+      <c r="X12">
+        <v>131</v>
+      </c>
+      <c r="Y12">
+        <v>205</v>
+      </c>
+      <c r="Z12">
+        <v>251</v>
+      </c>
+      <c r="AA12">
+        <v>429</v>
+      </c>
+      <c r="AB12">
+        <v>431</v>
+      </c>
+      <c r="AC12">
+        <v>252</v>
+      </c>
+      <c r="AD12">
+        <v>358</v>
+      </c>
+      <c r="AE12">
         <v>258</v>
       </c>
-      <c r="E12">
-        <v>363</v>
-      </c>
-      <c r="F12">
-        <v>433</v>
-      </c>
-      <c r="G12">
-        <v>468</v>
-      </c>
-      <c r="H12">
-        <v>468</v>
-      </c>
-      <c r="I12">
-        <v>433</v>
-      </c>
-      <c r="J12">
-        <v>363</v>
-      </c>
-      <c r="K12">
-        <v>258</v>
-      </c>
-      <c r="L12">
-        <v>335</v>
-      </c>
-      <c r="M12">
-        <v>242</v>
-      </c>
-      <c r="N12">
-        <v>233</v>
-      </c>
-      <c r="O12">
-        <v>173</v>
-      </c>
-      <c r="P12">
-        <v>203</v>
-      </c>
-      <c r="Q12">
-        <v>214</v>
-      </c>
-      <c r="R12">
-        <v>242</v>
-      </c>
-      <c r="S12">
-        <v>236</v>
-      </c>
-      <c r="T12">
-        <v>249</v>
-      </c>
-      <c r="U12">
-        <v>256</v>
-      </c>
-      <c r="V12">
-        <v>194</v>
-      </c>
-      <c r="W12">
-        <v>202</v>
-      </c>
-      <c r="X12">
+      <c r="AF12">
+        <v>218</v>
+      </c>
+      <c r="AG12">
+        <v>204</v>
+      </c>
+      <c r="AH12">
         <v>193</v>
       </c>
-      <c r="Y12">
-        <v>304</v>
-      </c>
-      <c r="Z12">
-        <v>258</v>
-      </c>
-      <c r="AA12">
-        <v>448</v>
-      </c>
-      <c r="AB12">
-        <v>448</v>
-      </c>
-      <c r="AC12">
-        <v>258</v>
-      </c>
-      <c r="AD12">
-        <v>372</v>
-      </c>
-      <c r="AE12">
-        <v>264</v>
-      </c>
-      <c r="AF12">
-        <v>229</v>
-      </c>
-      <c r="AG12">
-        <v>211</v>
-      </c>
-      <c r="AH12">
+      <c r="AI12">
         <v>199</v>
       </c>
-      <c r="AI12">
-        <v>203</v>
-      </c>
       <c r="AJ12">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="AK12">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AL12">
         <v>47</v>
@@ -1928,115 +1928,115 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D13">
-        <v>986</v>
+        <v>960</v>
       </c>
       <c r="E13">
-        <v>1389</v>
+        <v>1336</v>
       </c>
       <c r="F13">
-        <v>1657</v>
+        <v>1592</v>
       </c>
       <c r="G13">
-        <v>1791</v>
+        <v>1719</v>
       </c>
       <c r="H13">
-        <v>1791</v>
+        <v>1729</v>
       </c>
       <c r="I13">
-        <v>1657</v>
+        <v>1618</v>
       </c>
       <c r="J13">
-        <v>1389</v>
+        <v>1329</v>
       </c>
       <c r="K13">
-        <v>986</v>
+        <v>940</v>
       </c>
       <c r="L13">
-        <v>1270</v>
+        <v>858</v>
       </c>
       <c r="M13">
-        <v>1151</v>
+        <v>793</v>
       </c>
       <c r="N13">
+        <v>581</v>
+      </c>
+      <c r="O13">
+        <v>716</v>
+      </c>
+      <c r="P13">
+        <v>647</v>
+      </c>
+      <c r="Q13">
+        <v>537</v>
+      </c>
+      <c r="R13">
+        <v>681</v>
+      </c>
+      <c r="S13">
+        <v>572</v>
+      </c>
+      <c r="T13">
+        <v>607</v>
+      </c>
+      <c r="U13">
+        <v>511</v>
+      </c>
+      <c r="V13">
+        <v>551</v>
+      </c>
+      <c r="W13">
+        <v>575</v>
+      </c>
+      <c r="X13">
+        <v>684</v>
+      </c>
+      <c r="Y13">
         <v>857</v>
       </c>
-      <c r="O13">
-        <v>1055</v>
-      </c>
-      <c r="P13">
-        <v>963</v>
-      </c>
-      <c r="Q13">
-        <v>806</v>
-      </c>
-      <c r="R13">
-        <v>996</v>
-      </c>
-      <c r="S13">
-        <v>860</v>
-      </c>
-      <c r="T13">
-        <v>899</v>
-      </c>
-      <c r="U13">
-        <v>773</v>
-      </c>
-      <c r="V13">
-        <v>829</v>
-      </c>
-      <c r="W13">
-        <v>848</v>
-      </c>
-      <c r="X13">
-        <v>1019</v>
-      </c>
-      <c r="Y13">
-        <v>1267</v>
-      </c>
       <c r="Z13">
-        <v>986</v>
+        <v>947</v>
       </c>
       <c r="AA13">
-        <v>1717</v>
+        <v>1635</v>
       </c>
       <c r="AB13">
-        <v>1717</v>
+        <v>1664</v>
       </c>
       <c r="AC13">
-        <v>986</v>
+        <v>948</v>
       </c>
       <c r="AD13">
-        <v>1373</v>
+        <v>1338</v>
       </c>
       <c r="AE13">
-        <v>827</v>
+        <v>811</v>
       </c>
       <c r="AF13">
-        <v>854</v>
+        <v>814</v>
       </c>
       <c r="AG13">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="AH13">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="AI13">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="AJ13">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="AK13">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="AL13">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AM13">
         <v>23</v>
@@ -2050,109 +2050,109 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D14">
-        <v>780</v>
+        <v>743</v>
       </c>
       <c r="E14">
-        <v>1098</v>
+        <v>1050</v>
       </c>
       <c r="F14">
-        <v>1310</v>
+        <v>1277</v>
       </c>
       <c r="G14">
-        <v>1416</v>
+        <v>1378</v>
       </c>
       <c r="H14">
-        <v>1416</v>
+        <v>1363</v>
       </c>
       <c r="I14">
-        <v>1310</v>
+        <v>1275</v>
       </c>
       <c r="J14">
-        <v>1098</v>
+        <v>1054</v>
       </c>
       <c r="K14">
-        <v>780</v>
+        <v>749</v>
       </c>
       <c r="L14">
-        <v>1416</v>
+        <v>956</v>
       </c>
       <c r="M14">
-        <v>947</v>
+        <v>646</v>
       </c>
       <c r="N14">
-        <v>788</v>
+        <v>531</v>
       </c>
       <c r="O14">
-        <v>833</v>
+        <v>565</v>
       </c>
       <c r="P14">
-        <v>785</v>
+        <v>538</v>
       </c>
       <c r="Q14">
-        <v>780</v>
+        <v>520</v>
       </c>
       <c r="R14">
-        <v>864</v>
+        <v>575</v>
       </c>
       <c r="S14">
-        <v>749</v>
+        <v>494</v>
       </c>
       <c r="T14">
-        <v>479</v>
+        <v>328</v>
       </c>
       <c r="U14">
-        <v>564</v>
+        <v>375</v>
       </c>
       <c r="V14">
-        <v>589</v>
+        <v>393</v>
       </c>
       <c r="W14">
-        <v>630</v>
+        <v>428</v>
       </c>
       <c r="X14">
-        <v>714</v>
+        <v>474</v>
       </c>
       <c r="Y14">
-        <v>739</v>
+        <v>503</v>
       </c>
       <c r="Z14">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="AA14">
-        <v>1358</v>
+        <v>1303</v>
       </c>
       <c r="AB14">
-        <v>1358</v>
+        <v>1302</v>
       </c>
       <c r="AC14">
-        <v>780</v>
+        <v>741</v>
       </c>
       <c r="AD14">
-        <v>1171</v>
+        <v>1151</v>
       </c>
       <c r="AE14">
-        <v>655</v>
+        <v>639</v>
       </c>
       <c r="AF14">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="AG14">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="AH14">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="AI14">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="AJ14">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="AK14">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="AL14">
         <v>44</v>
@@ -2304,109 +2304,109 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2021</v>
+        <v>1944</v>
       </c>
       <c r="E2">
-        <v>2846</v>
+        <v>2762</v>
       </c>
       <c r="F2">
-        <v>3396</v>
+        <v>3312</v>
       </c>
       <c r="G2">
-        <v>3671</v>
+        <v>3533</v>
       </c>
       <c r="H2">
-        <v>3671</v>
+        <v>3546</v>
       </c>
       <c r="I2">
-        <v>3396</v>
+        <v>3265</v>
       </c>
       <c r="J2">
-        <v>2846</v>
+        <v>2705</v>
       </c>
       <c r="K2">
-        <v>2021</v>
+        <v>1973</v>
       </c>
       <c r="L2">
-        <v>593</v>
+        <v>410</v>
       </c>
       <c r="M2">
-        <v>696</v>
+        <v>476</v>
       </c>
       <c r="N2">
-        <v>619</v>
+        <v>419</v>
       </c>
       <c r="O2">
-        <v>816</v>
+        <v>552</v>
       </c>
       <c r="P2">
-        <v>835</v>
+        <v>559</v>
       </c>
       <c r="Q2">
-        <v>871</v>
+        <v>577</v>
       </c>
       <c r="R2">
-        <v>814</v>
+        <v>560</v>
       </c>
       <c r="S2">
-        <v>866</v>
+        <v>582</v>
       </c>
       <c r="T2">
-        <v>914</v>
+        <v>610</v>
       </c>
       <c r="U2">
-        <v>858</v>
+        <v>578</v>
       </c>
       <c r="V2">
-        <v>1171</v>
+        <v>778</v>
       </c>
       <c r="W2">
-        <v>1289</v>
+        <v>881</v>
       </c>
       <c r="X2">
-        <v>1714</v>
+        <v>1177</v>
       </c>
       <c r="Y2">
-        <v>1987</v>
+        <v>1323</v>
       </c>
       <c r="Z2">
-        <v>2021</v>
+        <v>1966</v>
       </c>
       <c r="AA2">
-        <v>3518</v>
+        <v>3440</v>
       </c>
       <c r="AB2">
-        <v>3518</v>
+        <v>3395</v>
       </c>
       <c r="AC2">
-        <v>2021</v>
+        <v>1953</v>
       </c>
       <c r="AD2">
-        <v>3671</v>
+        <v>3566</v>
       </c>
       <c r="AE2">
-        <v>3671</v>
+        <v>3527</v>
       </c>
       <c r="AF2">
-        <v>3631</v>
+        <v>3475</v>
       </c>
       <c r="AG2">
-        <v>3070</v>
+        <v>2930</v>
       </c>
       <c r="AH2">
-        <v>2320</v>
+        <v>2265</v>
       </c>
       <c r="AI2">
-        <v>2198</v>
+        <v>2133</v>
       </c>
       <c r="AJ2">
-        <v>1246</v>
+        <v>1211</v>
       </c>
       <c r="AK2">
-        <v>981</v>
+        <v>954</v>
       </c>
       <c r="AL2">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="AM2">
         <v>0</v>
@@ -2420,112 +2420,112 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="E3">
-        <v>547</v>
+        <v>528</v>
       </c>
       <c r="F3">
-        <v>653</v>
+        <v>626</v>
       </c>
       <c r="G3">
-        <v>706</v>
+        <v>672</v>
       </c>
       <c r="H3">
-        <v>706</v>
+        <v>675</v>
       </c>
       <c r="I3">
-        <v>653</v>
+        <v>626</v>
       </c>
       <c r="J3">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="K3">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="L3">
-        <v>682</v>
+        <v>460</v>
       </c>
       <c r="M3">
-        <v>528</v>
+        <v>352</v>
       </c>
       <c r="N3">
-        <v>482</v>
+        <v>321</v>
       </c>
       <c r="O3">
-        <v>454</v>
+        <v>303</v>
       </c>
       <c r="P3">
-        <v>470</v>
+        <v>324</v>
       </c>
       <c r="Q3">
-        <v>430</v>
+        <v>294</v>
       </c>
       <c r="R3">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="S3">
-        <v>462</v>
+        <v>315</v>
       </c>
       <c r="T3">
-        <v>373</v>
+        <v>250</v>
       </c>
       <c r="U3">
-        <v>372</v>
+        <v>251</v>
       </c>
       <c r="V3">
-        <v>342</v>
+        <v>232</v>
       </c>
       <c r="W3">
-        <v>326</v>
+        <v>221</v>
       </c>
       <c r="X3">
-        <v>305</v>
+        <v>208</v>
       </c>
       <c r="Y3">
-        <v>343</v>
+        <v>235</v>
       </c>
       <c r="Z3">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="AA3">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="AB3">
-        <v>676</v>
+        <v>657</v>
       </c>
       <c r="AC3">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="AD3">
-        <v>438</v>
+        <v>416</v>
       </c>
       <c r="AE3">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="AF3">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="AG3">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="AH3">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AI3">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AJ3">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AK3">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AL3">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AM3">
         <v>11</v>
@@ -2539,115 +2539,115 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E4">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="F4">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="G4">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="H4">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="I4">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="J4">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="K4">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="L4">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="M4">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="N4">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="O4">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="P4">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="Q4">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="R4">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="S4">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="T4">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="U4">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="V4">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="W4">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="X4">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="Y4">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="Z4">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="AA4">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="AB4">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="AC4">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AD4">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="AE4">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="AF4">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="AG4">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="AH4">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="AI4">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AJ4">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="AK4">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AL4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AM4">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:39">
@@ -2658,115 +2658,115 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E5">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="F5">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="G5">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="H5">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="I5">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="J5">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="K5">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="L5">
+        <v>80</v>
+      </c>
+      <c r="M5">
+        <v>75</v>
+      </c>
+      <c r="N5">
+        <v>75</v>
+      </c>
+      <c r="O5">
+        <v>61</v>
+      </c>
+      <c r="P5">
+        <v>69</v>
+      </c>
+      <c r="Q5">
+        <v>77</v>
+      </c>
+      <c r="R5">
+        <v>72</v>
+      </c>
+      <c r="S5">
+        <v>73</v>
+      </c>
+      <c r="T5">
+        <v>88</v>
+      </c>
+      <c r="U5">
+        <v>78</v>
+      </c>
+      <c r="V5">
+        <v>85</v>
+      </c>
+      <c r="W5">
+        <v>93</v>
+      </c>
+      <c r="X5">
         <v>115</v>
       </c>
-      <c r="M5">
-        <v>114</v>
-      </c>
-      <c r="N5">
-        <v>110</v>
-      </c>
-      <c r="O5">
-        <v>91</v>
-      </c>
-      <c r="P5">
-        <v>102</v>
-      </c>
-      <c r="Q5">
-        <v>112</v>
-      </c>
-      <c r="R5">
-        <v>108</v>
-      </c>
-      <c r="S5">
-        <v>109</v>
-      </c>
-      <c r="T5">
-        <v>133</v>
-      </c>
-      <c r="U5">
-        <v>117</v>
-      </c>
-      <c r="V5">
-        <v>127</v>
-      </c>
-      <c r="W5">
-        <v>135</v>
-      </c>
-      <c r="X5">
-        <v>166</v>
-      </c>
       <c r="Y5">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="Z5">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AA5">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="AB5">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="AC5">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AD5">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="AE5">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="AF5">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="AG5">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="AH5">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="AI5">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="AJ5">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AK5">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AL5">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AM5">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -2780,109 +2780,109 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E6">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F6">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G6">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="H6">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="I6">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="J6">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K6">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L6">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="M6">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="N6">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="O6">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="P6">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="Q6">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="R6">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="S6">
+        <v>52</v>
+      </c>
+      <c r="T6">
+        <v>54</v>
+      </c>
+      <c r="U6">
+        <v>59</v>
+      </c>
+      <c r="V6">
+        <v>53</v>
+      </c>
+      <c r="W6">
+        <v>54</v>
+      </c>
+      <c r="X6">
         <v>78</v>
       </c>
-      <c r="T6">
-        <v>80</v>
-      </c>
-      <c r="U6">
-        <v>89</v>
-      </c>
-      <c r="V6">
-        <v>79</v>
-      </c>
-      <c r="W6">
-        <v>81</v>
-      </c>
-      <c r="X6">
-        <v>114</v>
-      </c>
       <c r="Y6">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="Z6">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AA6">
+        <v>217</v>
+      </c>
+      <c r="AB6">
+        <v>212</v>
+      </c>
+      <c r="AC6">
+        <v>122</v>
+      </c>
+      <c r="AD6">
         <v>223</v>
       </c>
-      <c r="AB6">
-        <v>223</v>
-      </c>
-      <c r="AC6">
-        <v>128</v>
-      </c>
-      <c r="AD6">
-        <v>233</v>
-      </c>
       <c r="AE6">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="AF6">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AG6">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AH6">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AI6">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AJ6">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AK6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AL6">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AM6">
         <v>3</v>
@@ -2896,112 +2896,112 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="E7">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="F7">
-        <v>656</v>
+        <v>636</v>
       </c>
       <c r="G7">
-        <v>710</v>
+        <v>691</v>
       </c>
       <c r="H7">
-        <v>710</v>
+        <v>681</v>
       </c>
       <c r="I7">
-        <v>656</v>
+        <v>639</v>
       </c>
       <c r="J7">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="K7">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="L7">
-        <v>202</v>
+        <v>139</v>
       </c>
       <c r="M7">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="N7">
-        <v>222</v>
+        <v>147</v>
       </c>
       <c r="O7">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="P7">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="Q7">
-        <v>204</v>
+        <v>139</v>
       </c>
       <c r="R7">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="S7">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="T7">
-        <v>211</v>
+        <v>142</v>
       </c>
       <c r="U7">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="V7">
-        <v>273</v>
+        <v>185</v>
       </c>
       <c r="W7">
-        <v>311</v>
+        <v>210</v>
       </c>
       <c r="X7">
-        <v>355</v>
+        <v>243</v>
       </c>
       <c r="Y7">
-        <v>473</v>
+        <v>316</v>
       </c>
       <c r="Z7">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="AA7">
-        <v>680</v>
+        <v>665</v>
       </c>
       <c r="AB7">
-        <v>680</v>
+        <v>652</v>
       </c>
       <c r="AC7">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="AD7">
-        <v>710</v>
+        <v>681</v>
       </c>
       <c r="AE7">
-        <v>710</v>
+        <v>686</v>
       </c>
       <c r="AF7">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="AG7">
-        <v>465</v>
+        <v>443</v>
       </c>
       <c r="AH7">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="AI7">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="AJ7">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="AK7">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AL7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AM7">
         <v>5</v>
@@ -3015,112 +3015,112 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D8">
-        <v>619</v>
+        <v>600</v>
       </c>
       <c r="E8">
-        <v>871</v>
+        <v>829</v>
       </c>
       <c r="F8">
+        <v>993</v>
+      </c>
+      <c r="G8">
+        <v>1083</v>
+      </c>
+      <c r="H8">
+        <v>1086</v>
+      </c>
+      <c r="I8">
+        <v>1014</v>
+      </c>
+      <c r="J8">
+        <v>832</v>
+      </c>
+      <c r="K8">
+        <v>590</v>
+      </c>
+      <c r="L8">
+        <v>379</v>
+      </c>
+      <c r="M8">
+        <v>372</v>
+      </c>
+      <c r="N8">
+        <v>329</v>
+      </c>
+      <c r="O8">
+        <v>480</v>
+      </c>
+      <c r="P8">
+        <v>368</v>
+      </c>
+      <c r="Q8">
+        <v>359</v>
+      </c>
+      <c r="R8">
+        <v>274</v>
+      </c>
+      <c r="S8">
+        <v>336</v>
+      </c>
+      <c r="T8">
+        <v>357</v>
+      </c>
+      <c r="U8">
+        <v>347</v>
+      </c>
+      <c r="V8">
+        <v>355</v>
+      </c>
+      <c r="W8">
+        <v>377</v>
+      </c>
+      <c r="X8">
+        <v>440</v>
+      </c>
+      <c r="Y8">
+        <v>439</v>
+      </c>
+      <c r="Z8">
+        <v>604</v>
+      </c>
+      <c r="AA8">
+        <v>1027</v>
+      </c>
+      <c r="AB8">
         <v>1039</v>
       </c>
-      <c r="G8">
-        <v>1124</v>
-      </c>
-      <c r="H8">
-        <v>1124</v>
-      </c>
-      <c r="I8">
-        <v>1039</v>
-      </c>
-      <c r="J8">
-        <v>871</v>
-      </c>
-      <c r="K8">
-        <v>619</v>
-      </c>
-      <c r="L8">
-        <v>560</v>
-      </c>
-      <c r="M8">
-        <v>559</v>
-      </c>
-      <c r="N8">
-        <v>489</v>
-      </c>
-      <c r="O8">
-        <v>709</v>
-      </c>
-      <c r="P8">
-        <v>542</v>
-      </c>
-      <c r="Q8">
-        <v>540</v>
-      </c>
-      <c r="R8">
-        <v>410</v>
-      </c>
-      <c r="S8">
-        <v>498</v>
-      </c>
-      <c r="T8">
-        <v>536</v>
-      </c>
-      <c r="U8">
-        <v>514</v>
-      </c>
-      <c r="V8">
-        <v>537</v>
-      </c>
-      <c r="W8">
-        <v>550</v>
-      </c>
-      <c r="X8">
-        <v>637</v>
-      </c>
-      <c r="Y8">
-        <v>661</v>
-      </c>
-      <c r="Z8">
-        <v>619</v>
-      </c>
-      <c r="AA8">
-        <v>1077</v>
-      </c>
-      <c r="AB8">
-        <v>1077</v>
-      </c>
       <c r="AC8">
-        <v>619</v>
+        <v>596</v>
       </c>
       <c r="AD8">
-        <v>1124</v>
+        <v>1087</v>
       </c>
       <c r="AE8">
-        <v>747</v>
+        <v>730</v>
       </c>
       <c r="AF8">
-        <v>609</v>
+        <v>576</v>
       </c>
       <c r="AG8">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="AH8">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="AI8">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="AJ8">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="AK8">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="AL8">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AM8">
         <v>9</v>
@@ -3134,112 +3134,112 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E9">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F9">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="G9">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="H9">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="I9">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="J9">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="K9">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="L9">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="M9">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="N9">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="O9">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="P9">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="Q9">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="R9">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="S9">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="T9">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="U9">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="V9">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="W9">
+        <v>127</v>
+      </c>
+      <c r="X9">
+        <v>149</v>
+      </c>
+      <c r="Y9">
+        <v>183</v>
+      </c>
+      <c r="Z9">
+        <v>218</v>
+      </c>
+      <c r="AA9">
+        <v>385</v>
+      </c>
+      <c r="AB9">
+        <v>389</v>
+      </c>
+      <c r="AC9">
+        <v>222</v>
+      </c>
+      <c r="AD9">
+        <v>398</v>
+      </c>
+      <c r="AE9">
+        <v>395</v>
+      </c>
+      <c r="AF9">
+        <v>260</v>
+      </c>
+      <c r="AG9">
         <v>189</v>
       </c>
-      <c r="X9">
-        <v>219</v>
-      </c>
-      <c r="Y9">
-        <v>272</v>
-      </c>
-      <c r="Z9">
-        <v>229</v>
-      </c>
-      <c r="AA9">
-        <v>398</v>
-      </c>
-      <c r="AB9">
-        <v>398</v>
-      </c>
-      <c r="AC9">
-        <v>229</v>
-      </c>
-      <c r="AD9">
-        <v>416</v>
-      </c>
-      <c r="AE9">
-        <v>414</v>
-      </c>
-      <c r="AF9">
-        <v>274</v>
-      </c>
-      <c r="AG9">
-        <v>195</v>
-      </c>
       <c r="AH9">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AI9">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AJ9">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AK9">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="AL9">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AM9">
         <v>3</v>
@@ -3253,115 +3253,115 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D10">
-        <v>954</v>
+        <v>909</v>
       </c>
       <c r="E10">
-        <v>1343</v>
+        <v>1300</v>
       </c>
       <c r="F10">
-        <v>1603</v>
+        <v>1548</v>
       </c>
       <c r="G10">
-        <v>1733</v>
+        <v>1653</v>
       </c>
       <c r="H10">
-        <v>1733</v>
+        <v>1677</v>
       </c>
       <c r="I10">
-        <v>1603</v>
+        <v>1525</v>
       </c>
       <c r="J10">
-        <v>1343</v>
+        <v>1303</v>
       </c>
       <c r="K10">
-        <v>954</v>
+        <v>920</v>
       </c>
       <c r="L10">
-        <v>1230</v>
+        <v>846</v>
       </c>
       <c r="M10">
-        <v>1124</v>
+        <v>764</v>
       </c>
       <c r="N10">
-        <v>1099</v>
+        <v>726</v>
       </c>
       <c r="O10">
-        <v>1014</v>
+        <v>685</v>
       </c>
       <c r="P10">
-        <v>1123</v>
+        <v>757</v>
       </c>
       <c r="Q10">
-        <v>1080</v>
+        <v>730</v>
       </c>
       <c r="R10">
-        <v>1069</v>
+        <v>728</v>
       </c>
       <c r="S10">
-        <v>973</v>
+        <v>663</v>
       </c>
       <c r="T10">
-        <v>1032</v>
+        <v>698</v>
       </c>
       <c r="U10">
-        <v>1001</v>
+        <v>674</v>
       </c>
       <c r="V10">
-        <v>960</v>
+        <v>640</v>
       </c>
       <c r="W10">
-        <v>867</v>
+        <v>593</v>
       </c>
       <c r="X10">
-        <v>1002</v>
+        <v>680</v>
       </c>
       <c r="Y10">
-        <v>979</v>
+        <v>658</v>
       </c>
       <c r="Z10">
-        <v>954</v>
+        <v>917</v>
       </c>
       <c r="AA10">
-        <v>1660</v>
+        <v>1611</v>
       </c>
       <c r="AB10">
-        <v>1660</v>
+        <v>1613</v>
       </c>
       <c r="AC10">
-        <v>954</v>
+        <v>913</v>
       </c>
       <c r="AD10">
-        <v>1133</v>
+        <v>1065</v>
       </c>
       <c r="AE10">
-        <v>814</v>
+        <v>785</v>
       </c>
       <c r="AF10">
-        <v>656</v>
+        <v>632</v>
       </c>
       <c r="AG10">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="AH10">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="AI10">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="AJ10">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AK10">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL10">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AM10">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:39">
@@ -3375,109 +3375,109 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E11">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F11">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G11">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H11">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I11">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J11">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K11">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L11">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="M11">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>46</v>
+      </c>
+      <c r="P11">
+        <v>49</v>
+      </c>
+      <c r="Q11">
+        <v>47</v>
+      </c>
+      <c r="R11">
+        <v>49</v>
+      </c>
+      <c r="S11">
+        <v>56</v>
+      </c>
+      <c r="T11">
+        <v>50</v>
+      </c>
+      <c r="U11">
+        <v>52</v>
+      </c>
+      <c r="V11">
+        <v>49</v>
+      </c>
+      <c r="W11">
+        <v>63</v>
+      </c>
+      <c r="X11">
+        <v>58</v>
+      </c>
+      <c r="Y11">
         <v>75</v>
       </c>
-      <c r="O11">
+      <c r="Z11">
+        <v>85</v>
+      </c>
+      <c r="AA11">
+        <v>146</v>
+      </c>
+      <c r="AB11">
+        <v>147</v>
+      </c>
+      <c r="AC11">
+        <v>85</v>
+      </c>
+      <c r="AD11">
+        <v>133</v>
+      </c>
+      <c r="AE11">
+        <v>110</v>
+      </c>
+      <c r="AF11">
         <v>68</v>
       </c>
-      <c r="P11">
-        <v>73</v>
-      </c>
-      <c r="Q11">
+      <c r="AG11">
         <v>70</v>
       </c>
-      <c r="R11">
-        <v>72</v>
-      </c>
-      <c r="S11">
-        <v>82</v>
-      </c>
-      <c r="T11">
-        <v>76</v>
-      </c>
-      <c r="U11">
-        <v>78</v>
-      </c>
-      <c r="V11">
-        <v>73</v>
-      </c>
-      <c r="W11">
-        <v>93</v>
-      </c>
-      <c r="X11">
-        <v>86</v>
-      </c>
-      <c r="Y11">
-        <v>110</v>
-      </c>
-      <c r="Z11">
-        <v>88</v>
-      </c>
-      <c r="AA11">
-        <v>153</v>
-      </c>
-      <c r="AB11">
-        <v>153</v>
-      </c>
-      <c r="AC11">
-        <v>88</v>
-      </c>
-      <c r="AD11">
-        <v>141</v>
-      </c>
-      <c r="AE11">
-        <v>111</v>
-      </c>
-      <c r="AF11">
-        <v>72</v>
-      </c>
-      <c r="AG11">
-        <v>73</v>
-      </c>
       <c r="AH11">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AI11">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AJ11">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AK11">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AL11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AM11">
         <v>4</v>
@@ -3494,103 +3494,103 @@
         <v>3</v>
       </c>
       <c r="D12">
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <v>63</v>
+      </c>
+      <c r="F12">
+        <v>75</v>
+      </c>
+      <c r="G12">
+        <v>82</v>
+      </c>
+      <c r="H12">
+        <v>82</v>
+      </c>
+      <c r="I12">
+        <v>76</v>
+      </c>
+      <c r="J12">
+        <v>64</v>
+      </c>
+      <c r="K12">
+        <v>44</v>
+      </c>
+      <c r="L12">
+        <v>42</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="N12">
+        <v>28</v>
+      </c>
+      <c r="O12">
+        <v>21</v>
+      </c>
+      <c r="P12">
+        <v>25</v>
+      </c>
+      <c r="Q12">
+        <v>26</v>
+      </c>
+      <c r="R12">
+        <v>30</v>
+      </c>
+      <c r="S12">
+        <v>28</v>
+      </c>
+      <c r="T12">
+        <v>30</v>
+      </c>
+      <c r="U12">
+        <v>31</v>
+      </c>
+      <c r="V12">
+        <v>23</v>
+      </c>
+      <c r="W12">
+        <v>25</v>
+      </c>
+      <c r="X12">
+        <v>24</v>
+      </c>
+      <c r="Y12">
+        <v>37</v>
+      </c>
+      <c r="Z12">
+        <v>45</v>
+      </c>
+      <c r="AA12">
+        <v>78</v>
+      </c>
+      <c r="AB12">
+        <v>79</v>
+      </c>
+      <c r="AC12">
+        <v>45</v>
+      </c>
+      <c r="AD12">
+        <v>65</v>
+      </c>
+      <c r="AE12">
         <v>46</v>
       </c>
-      <c r="E12">
-        <v>65</v>
-      </c>
-      <c r="F12">
-        <v>78</v>
-      </c>
-      <c r="G12">
-        <v>84</v>
-      </c>
-      <c r="H12">
-        <v>84</v>
-      </c>
-      <c r="I12">
-        <v>78</v>
-      </c>
-      <c r="J12">
-        <v>65</v>
-      </c>
-      <c r="K12">
-        <v>46</v>
-      </c>
-      <c r="L12">
-        <v>61</v>
-      </c>
-      <c r="M12">
-        <v>45</v>
-      </c>
-      <c r="N12">
-        <v>42</v>
-      </c>
-      <c r="O12">
-        <v>31</v>
-      </c>
-      <c r="P12">
+      <c r="AF12">
+        <v>40</v>
+      </c>
+      <c r="AG12">
         <v>37</v>
-      </c>
-      <c r="Q12">
-        <v>39</v>
-      </c>
-      <c r="R12">
-        <v>43</v>
-      </c>
-      <c r="S12">
-        <v>42</v>
-      </c>
-      <c r="T12">
-        <v>45</v>
-      </c>
-      <c r="U12">
-        <v>47</v>
-      </c>
-      <c r="V12">
-        <v>35</v>
-      </c>
-      <c r="W12">
-        <v>36</v>
-      </c>
-      <c r="X12">
-        <v>35</v>
-      </c>
-      <c r="Y12">
-        <v>55</v>
-      </c>
-      <c r="Z12">
-        <v>46</v>
-      </c>
-      <c r="AA12">
-        <v>81</v>
-      </c>
-      <c r="AB12">
-        <v>81</v>
-      </c>
-      <c r="AC12">
-        <v>46</v>
-      </c>
-      <c r="AD12">
-        <v>68</v>
-      </c>
-      <c r="AE12">
-        <v>47</v>
-      </c>
-      <c r="AF12">
-        <v>41</v>
-      </c>
-      <c r="AG12">
-        <v>38</v>
       </c>
       <c r="AH12">
         <v>35</v>
       </c>
       <c r="AI12">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AJ12">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AK12">
         <v>18</v>
@@ -3613,103 +3613,103 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H13">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I13">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J13">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L13">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="M13">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="N13">
+        <v>17</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>14</v>
+      </c>
+      <c r="Q13">
+        <v>17</v>
+      </c>
+      <c r="R13">
+        <v>17</v>
+      </c>
+      <c r="S13">
+        <v>16</v>
+      </c>
+      <c r="T13">
+        <v>16</v>
+      </c>
+      <c r="U13">
+        <v>14</v>
+      </c>
+      <c r="V13">
+        <v>14</v>
+      </c>
+      <c r="W13">
+        <v>18</v>
+      </c>
+      <c r="X13">
+        <v>21</v>
+      </c>
+      <c r="Y13">
         <v>26</v>
       </c>
-      <c r="O13">
+      <c r="Z13">
+        <v>31</v>
+      </c>
+      <c r="AA13">
+        <v>52</v>
+      </c>
+      <c r="AB13">
+        <v>54</v>
+      </c>
+      <c r="AC13">
+        <v>30</v>
+      </c>
+      <c r="AD13">
+        <v>56</v>
+      </c>
+      <c r="AE13">
+        <v>43</v>
+      </c>
+      <c r="AF13">
+        <v>37</v>
+      </c>
+      <c r="AG13">
         <v>24</v>
-      </c>
-      <c r="P13">
-        <v>21</v>
-      </c>
-      <c r="Q13">
-        <v>25</v>
-      </c>
-      <c r="R13">
-        <v>25</v>
-      </c>
-      <c r="S13">
-        <v>23</v>
-      </c>
-      <c r="T13">
-        <v>23</v>
-      </c>
-      <c r="U13">
-        <v>21</v>
-      </c>
-      <c r="V13">
-        <v>20</v>
-      </c>
-      <c r="W13">
-        <v>27</v>
-      </c>
-      <c r="X13">
-        <v>31</v>
-      </c>
-      <c r="Y13">
-        <v>39</v>
-      </c>
-      <c r="Z13">
-        <v>32</v>
-      </c>
-      <c r="AA13">
-        <v>55</v>
-      </c>
-      <c r="AB13">
-        <v>55</v>
-      </c>
-      <c r="AC13">
-        <v>32</v>
-      </c>
-      <c r="AD13">
-        <v>58</v>
-      </c>
-      <c r="AE13">
-        <v>44</v>
-      </c>
-      <c r="AF13">
-        <v>39</v>
-      </c>
-      <c r="AG13">
-        <v>25</v>
       </c>
       <c r="AH13">
         <v>26</v>
       </c>
       <c r="AI13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AJ13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AK13">
         <v>11</v>

</xml_diff>